<commit_message>
Auto-committed on 2022/04/18 週一
</commit_message>
<xml_diff>
--- a/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L4-批次作業/PostAuthLog.xlsx
+++ b/Program/Other/Sharepoint上傳用/URS會議審查紀錄/DbLayouts/L4-批次作業/PostAuthLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\SKL\DB\GenTables\L4-批次作業\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SKL\DB\GenTables\L4-批次作業\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBB3669-5DC8-4C30-A97E-3518E726B1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFD2AED-0F7C-4CDE-B244-F95007502E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="2064" windowWidth="21840" windowHeight="10896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DBD" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="251">
   <si>
     <t>SEQ</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1951,13 +1951,6 @@
 1:需審查/確認
 2:為凍結名單/未確定名單</t>
     <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ProcessTime</t>
-  </si>
-  <si>
-    <t>處理時間</t>
-    <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
     <t>授權類別</t>
@@ -2265,7 +2258,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2422,9 +2415,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2470,41 +2460,41 @@
     <xf numFmtId="49" fontId="7" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2846,10 +2836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.44140625" defaultRowHeight="16.2"/>
@@ -2864,10 +2854,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="66"/>
+      <c r="B1" s="65"/>
       <c r="C1" s="3" t="s">
         <v>229</v>
       </c>
@@ -2879,8 +2869,8 @@
       <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="65"/>
-      <c r="B2" s="66"/>
+      <c r="A2" s="64"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="8" t="s">
         <v>110</v>
       </c>
@@ -2892,10 +2882,10 @@
       <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="48.6">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="64"/>
+      <c r="B3" s="63"/>
       <c r="C3" s="12" t="s">
         <v>52</v>
       </c>
@@ -2907,10 +2897,10 @@
       <c r="G3" s="11"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="67"/>
+      <c r="B4" s="66"/>
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
       <c r="E4" s="10"/>
@@ -2918,10 +2908,10 @@
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="64"/>
+      <c r="B5" s="63"/>
       <c r="C5" s="18" t="s">
         <v>63</v>
       </c>
@@ -2931,10 +2921,10 @@
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="66"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="44" t="s">
         <v>93</v>
       </c>
@@ -2944,10 +2934,10 @@
       <c r="G6" s="11"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="67"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="18" t="s">
         <v>64</v>
       </c>
@@ -2957,10 +2947,10 @@
       <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="64"/>
+      <c r="B8" s="63"/>
       <c r="C8" s="18" t="s">
         <v>65</v>
       </c>
@@ -3093,8 +3083,8 @@
       <c r="B15" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="53" t="s">
-        <v>247</v>
+      <c r="C15" s="52" t="s">
+        <v>245</v>
       </c>
       <c r="D15" s="44" t="s">
         <v>19</v>
@@ -3143,26 +3133,26 @@
       <c r="G17" s="50"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="60">
+      <c r="A18" s="59">
         <v>9</v>
       </c>
-      <c r="B18" s="63" t="s">
-        <v>251</v>
-      </c>
-      <c r="C18" s="61" t="s">
-        <v>252</v>
-      </c>
-      <c r="D18" s="62" t="s">
+      <c r="B18" s="62" t="s">
+        <v>249</v>
+      </c>
+      <c r="C18" s="60" t="s">
+        <v>250</v>
+      </c>
+      <c r="D18" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="60">
+      <c r="E18" s="59">
         <v>8</v>
       </c>
-      <c r="F18" s="59"/>
+      <c r="F18" s="58"/>
       <c r="G18" s="50"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="60">
+      <c r="A19" s="59">
         <v>10</v>
       </c>
       <c r="B19" s="45" t="s">
@@ -3180,7 +3170,7 @@
       <c r="G19" s="50"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="60">
+      <c r="A20" s="59">
         <v>11</v>
       </c>
       <c r="B20" s="45" t="s">
@@ -3189,41 +3179,39 @@
       <c r="C20" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="D20" s="48" t="s">
+      <c r="D20" s="61" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" s="49"/>
+      <c r="G20" s="50"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="59">
+        <v>12</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E21" s="49">
         <v>8</v>
       </c>
-      <c r="G20" s="50"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="60">
-        <v>12</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>245</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="D21" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="16">
-        <v>6</v>
-      </c>
-      <c r="G21" s="52"/>
+      <c r="G21" s="50"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="60">
+      <c r="A22" s="59">
         <v>13</v>
       </c>
       <c r="B22" s="45" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="C22" s="45" t="s">
-        <v>76</v>
+        <v>28</v>
       </c>
       <c r="D22" s="48" t="s">
         <v>55</v>
@@ -3233,33 +3221,35 @@
       </c>
       <c r="G22" s="50"/>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="60">
+    <row r="23" spans="1:7" ht="97.2">
+      <c r="A23" s="59">
         <v>14</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>32</v>
+        <v>94</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="49">
-        <v>8</v>
-      </c>
-      <c r="G23" s="50"/>
-    </row>
-    <row r="24" spans="1:7" ht="97.2">
-      <c r="A24" s="60">
+        <v>119</v>
+      </c>
+      <c r="D23" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="46">
+        <v>1</v>
+      </c>
+      <c r="G23" s="21" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="32.4">
+      <c r="A24" s="59">
         <v>15</v>
       </c>
-      <c r="B24" s="45" t="s">
-        <v>94</v>
+      <c r="B24" s="44" t="s">
+        <v>83</v>
       </c>
       <c r="C24" s="45" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D24" s="44" t="s">
         <v>19</v>
@@ -3267,100 +3257,100 @@
       <c r="E24" s="46">
         <v>1</v>
       </c>
-      <c r="G24" s="21" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="32.4">
-      <c r="A25" s="60">
+      <c r="G24" s="22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="324">
+      <c r="A25" s="59">
         <v>16</v>
       </c>
       <c r="B25" s="44" t="s">
-        <v>83</v>
+        <v>232</v>
       </c>
       <c r="C25" s="45" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="D25" s="44" t="s">
         <v>19</v>
       </c>
       <c r="E25" s="46">
+        <v>2</v>
+      </c>
+      <c r="G25" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="81">
+      <c r="A26" s="59">
+        <v>17</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>246</v>
+      </c>
+      <c r="C26" s="52" t="s">
+        <v>247</v>
+      </c>
+      <c r="D26" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="55">
         <v>1</v>
       </c>
-      <c r="G25" s="22" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="324">
-      <c r="A26" s="60">
-        <v>17</v>
-      </c>
-      <c r="B26" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="C26" s="45" t="s">
-        <v>102</v>
-      </c>
-      <c r="D26" s="44" t="s">
+      <c r="F26" s="56"/>
+      <c r="G26" s="57" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="59">
+        <v>18</v>
+      </c>
+      <c r="B27" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="46">
+        <v>6</v>
+      </c>
+      <c r="G27" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="59">
         <v>19</v>
       </c>
-      <c r="E26" s="46">
-        <v>2</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="81">
-      <c r="A27" s="60">
-        <v>18</v>
-      </c>
-      <c r="B27" s="54" t="s">
-        <v>248</v>
-      </c>
-      <c r="C27" s="53" t="s">
-        <v>249</v>
-      </c>
-      <c r="D27" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" s="56">
-        <v>1</v>
-      </c>
-      <c r="F27" s="57"/>
-      <c r="G27" s="58" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="60">
-        <v>19</v>
-      </c>
       <c r="B28" s="44" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C28" s="45" t="s">
-        <v>97</v>
+        <v>36</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>39</v>
-      </c>
-      <c r="E28" s="46">
-        <v>6</v>
-      </c>
-      <c r="G28" s="21" t="s">
-        <v>101</v>
+        <v>55</v>
+      </c>
+      <c r="E28" s="49">
+        <v>8</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="60">
+      <c r="A29" s="59">
         <v>20</v>
       </c>
       <c r="B29" s="44" t="s">
-        <v>96</v>
+        <v>34</v>
       </c>
       <c r="C29" s="45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D29" s="48" t="s">
         <v>55</v>
@@ -3368,19 +3358,17 @@
       <c r="E29" s="49">
         <v>8</v>
       </c>
-      <c r="G29" s="20" t="s">
-        <v>99</v>
-      </c>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="60">
+      <c r="A30" s="59">
         <v>21</v>
       </c>
       <c r="B30" s="44" t="s">
-        <v>34</v>
+        <v>225</v>
       </c>
       <c r="C30" s="45" t="s">
-        <v>37</v>
+        <v>228</v>
       </c>
       <c r="D30" s="48" t="s">
         <v>55</v>
@@ -3390,226 +3378,208 @@
       </c>
       <c r="G30" s="20"/>
     </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="60">
+    <row r="31" spans="1:7" ht="226.8">
+      <c r="A31" s="59">
         <v>22</v>
       </c>
       <c r="B31" s="44" t="s">
-        <v>225</v>
+        <v>35</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>228</v>
-      </c>
-      <c r="D31" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="46">
+        <v>2</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="59">
+        <v>23</v>
+      </c>
+      <c r="B32" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="46">
+        <v>100</v>
+      </c>
+      <c r="G32" s="20"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="59">
+        <v>24</v>
+      </c>
+      <c r="B33" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="46">
+        <v>10</v>
+      </c>
+      <c r="G33" s="24"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="59">
+        <v>25</v>
+      </c>
+      <c r="B34" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="49">
+      <c r="E34" s="49">
         <v>8</v>
       </c>
-      <c r="G31" s="20"/>
-    </row>
-    <row r="32" spans="1:7" ht="226.8">
-      <c r="A32" s="60">
-        <v>23</v>
-      </c>
-      <c r="B32" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="44" t="s">
+      <c r="G34" s="20"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="59">
+        <v>26</v>
+      </c>
+      <c r="B35" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E32" s="46">
-        <v>2</v>
-      </c>
-      <c r="G32" s="23" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="60">
-        <v>24</v>
-      </c>
-      <c r="B33" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" s="44" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" s="46">
-        <v>100</v>
-      </c>
-      <c r="G33" s="20"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="60">
-        <v>25</v>
-      </c>
-      <c r="B34" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="C34" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="D34" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="E34" s="46">
-        <v>10</v>
-      </c>
-      <c r="G34" s="24"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="60">
-        <v>26</v>
-      </c>
-      <c r="B35" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="C35" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="49">
-        <v>8</v>
-      </c>
-      <c r="G35" s="20"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="60">
+      <c r="E35" s="46">
+        <v>1</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="64.8">
+      <c r="A36" s="59">
         <v>27</v>
       </c>
       <c r="B36" s="44" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
       <c r="C36" s="45" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D36" s="44" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="E36" s="46">
         <v>1</v>
       </c>
-      <c r="G36" s="20" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="64.8">
-      <c r="A37" s="60">
+      <c r="G36" s="23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="59">
         <v>28</v>
       </c>
       <c r="B37" s="44" t="s">
-        <v>77</v>
+        <v>234</v>
       </c>
       <c r="C37" s="45" t="s">
-        <v>75</v>
+        <v>235</v>
       </c>
       <c r="D37" s="44" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="E37" s="46">
-        <v>1</v>
-      </c>
-      <c r="G37" s="23" t="s">
-        <v>244</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="G37" s="47"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="60">
+      <c r="A38" s="59">
         <v>29</v>
       </c>
       <c r="B38" s="44" t="s">
-        <v>234</v>
+        <v>69</v>
       </c>
       <c r="C38" s="45" t="s">
-        <v>235</v>
+        <v>70</v>
       </c>
       <c r="D38" s="44" t="s">
         <v>19</v>
       </c>
       <c r="E38" s="46">
-        <v>5</v>
-      </c>
-      <c r="G38" s="47"/>
+        <v>6</v>
+      </c>
+      <c r="G38" s="20"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="60">
+      <c r="A39" s="59">
         <v>30</v>
       </c>
       <c r="B39" s="44" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="C39" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="D39" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" s="49"/>
+      <c r="G39" s="20"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="59">
+        <v>31</v>
+      </c>
+      <c r="B40" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="46">
+      <c r="E40" s="46">
         <v>6</v>
       </c>
-      <c r="G39" s="20"/>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="60">
-        <v>31</v>
-      </c>
-      <c r="B40" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="C40" s="45" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" s="48" t="s">
+      <c r="G40" s="20"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="59">
+        <v>32</v>
+      </c>
+      <c r="B41" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="E40" s="49"/>
-      <c r="G40" s="20"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="60">
-        <v>32</v>
-      </c>
-      <c r="B41" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="D41" s="44" t="s">
-        <v>19</v>
-      </c>
-      <c r="E41" s="46">
-        <v>6</v>
-      </c>
+      <c r="E41" s="49"/>
       <c r="G41" s="20"/>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="60">
-        <v>33</v>
-      </c>
-      <c r="B42" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="C42" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="D42" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="E42" s="49"/>
-      <c r="G42" s="20"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="B43" s="46"/>
+      <c r="B42" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3860,32 +3830,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="69" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="25"/>
@@ -3912,10 +3882,10 @@
       <c r="D4" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="E4" s="79" t="s">
+      <c r="E4" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="F4" s="79"/>
+      <c r="F4" s="70"/>
       <c r="G4" s="29" t="s">
         <v>131</v>
       </c>
@@ -3942,10 +3912,10 @@
       <c r="D5" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="E5" s="74" t="s">
+      <c r="E5" s="67" t="s">
         <v>137</v>
       </c>
-      <c r="F5" s="74"/>
+      <c r="F5" s="67"/>
       <c r="G5" s="32">
         <v>1</v>
       </c>
@@ -3972,10 +3942,10 @@
       <c r="D6" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="E6" s="74" t="s">
+      <c r="E6" s="67" t="s">
         <v>141</v>
       </c>
-      <c r="F6" s="74"/>
+      <c r="F6" s="67"/>
       <c r="G6" s="32">
         <v>846</v>
       </c>
@@ -4002,10 +3972,10 @@
       <c r="D7" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="E7" s="74" t="s">
+      <c r="E7" s="67" t="s">
         <v>146</v>
       </c>
-      <c r="F7" s="74"/>
+      <c r="F7" s="67"/>
       <c r="G7" s="34" t="s">
         <v>147</v>
       </c>
@@ -4032,10 +4002,10 @@
       <c r="D8" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="E8" s="74" t="s">
+      <c r="E8" s="67" t="s">
         <v>151</v>
       </c>
-      <c r="F8" s="74"/>
+      <c r="F8" s="67"/>
       <c r="G8" s="32" t="s">
         <v>152</v>
       </c>
@@ -4062,10 +4032,10 @@
       <c r="D9" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="E9" s="74" t="s">
+      <c r="E9" s="67" t="s">
         <v>156</v>
       </c>
-      <c r="F9" s="74"/>
+      <c r="F9" s="67"/>
       <c r="G9" s="35" t="s">
         <v>157</v>
       </c>
@@ -4092,10 +4062,10 @@
       <c r="D10" s="30" t="s">
         <v>161</v>
       </c>
-      <c r="E10" s="74" t="s">
+      <c r="E10" s="67" t="s">
         <v>162</v>
       </c>
-      <c r="F10" s="74"/>
+      <c r="F10" s="67"/>
       <c r="G10" s="36" t="s">
         <v>163</v>
       </c>
@@ -4154,10 +4124,10 @@
       <c r="D12" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="67" t="s">
         <v>170</v>
       </c>
-      <c r="F12" s="74"/>
+      <c r="F12" s="67"/>
       <c r="G12" s="32" t="s">
         <v>171</v>
       </c>
@@ -4172,52 +4142,52 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="76">
+      <c r="A13" s="71">
         <v>9</v>
       </c>
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="76" t="s">
+      <c r="C13" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="76" t="s">
+      <c r="D13" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="E13" s="74" t="s">
+      <c r="E13" s="67" t="s">
         <v>174</v>
       </c>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72" t="s">
+      <c r="F13" s="67"/>
+      <c r="G13" s="73" t="s">
         <v>175</v>
       </c>
-      <c r="H13" s="72" t="s">
+      <c r="H13" s="73" t="s">
         <v>175</v>
       </c>
-      <c r="I13" s="72" t="s">
+      <c r="I13" s="73" t="s">
         <v>175</v>
       </c>
-      <c r="J13" s="72" t="s">
+      <c r="J13" s="73" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="76"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="74" t="s">
+      <c r="A14" s="71"/>
+      <c r="B14" s="67"/>
+      <c r="C14" s="71"/>
+      <c r="D14" s="71"/>
+      <c r="E14" s="67" t="s">
         <v>176</v>
       </c>
-      <c r="F14" s="74"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73" t="s">
+      <c r="F14" s="67"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74" t="s">
         <v>175</v>
       </c>
-      <c r="I14" s="73" t="s">
+      <c r="I14" s="74" t="s">
         <v>177</v>
       </c>
-      <c r="J14" s="73"/>
+      <c r="J14" s="74"/>
     </row>
     <row r="15" spans="1:10" ht="31.8">
       <c r="A15" s="30">
@@ -4232,10 +4202,10 @@
       <c r="D15" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="67" t="s">
         <v>181</v>
       </c>
-      <c r="F15" s="74"/>
+      <c r="F15" s="67"/>
       <c r="G15" s="32" t="s">
         <v>182</v>
       </c>
@@ -4262,10 +4232,10 @@
       <c r="D16" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="E16" s="74" t="s">
+      <c r="E16" s="67" t="s">
         <v>186</v>
       </c>
-      <c r="F16" s="74"/>
+      <c r="F16" s="67"/>
       <c r="G16" s="32" t="s">
         <v>187</v>
       </c>
@@ -4292,10 +4262,10 @@
       <c r="D17" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="E17" s="74" t="s">
+      <c r="E17" s="67" t="s">
         <v>191</v>
       </c>
-      <c r="F17" s="74"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="32" t="s">
         <v>192</v>
       </c>
@@ -4322,10 +4292,10 @@
       <c r="D18" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="E18" s="74" t="s">
+      <c r="E18" s="67" t="s">
         <v>191</v>
       </c>
-      <c r="F18" s="74"/>
+      <c r="F18" s="67"/>
       <c r="G18" s="32" t="s">
         <v>192</v>
       </c>
@@ -4352,10 +4322,10 @@
       <c r="D19" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="E19" s="74" t="s">
+      <c r="E19" s="67" t="s">
         <v>146</v>
       </c>
-      <c r="F19" s="74"/>
+      <c r="F19" s="67"/>
       <c r="G19" s="32" t="s">
         <v>192</v>
       </c>
@@ -4462,10 +4432,10 @@
       <c r="D25" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="E25" s="70" t="s">
+      <c r="E25" s="72" t="s">
         <v>198</v>
       </c>
-      <c r="F25" s="70"/>
+      <c r="F25" s="72"/>
       <c r="G25" s="41">
         <v>2</v>
       </c>
@@ -4492,10 +4462,10 @@
       <c r="D26" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="E26" s="70" t="s">
+      <c r="E26" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="F26" s="70"/>
+      <c r="F26" s="72"/>
       <c r="G26" s="41">
         <v>846</v>
       </c>
@@ -4522,10 +4492,10 @@
       <c r="D27" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="E27" s="70" t="s">
+      <c r="E27" s="72" t="s">
         <v>202</v>
       </c>
-      <c r="F27" s="70"/>
+      <c r="F27" s="72"/>
       <c r="G27" s="41" t="s">
         <v>192</v>
       </c>
@@ -4552,10 +4522,10 @@
       <c r="D28" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="E28" s="70" t="s">
+      <c r="E28" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="F28" s="70"/>
+      <c r="F28" s="72"/>
       <c r="G28" s="32" t="s">
         <v>152</v>
       </c>
@@ -4582,10 +4552,10 @@
       <c r="D29" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="E29" s="70" t="s">
+      <c r="E29" s="72" t="s">
         <v>200</v>
       </c>
-      <c r="F29" s="70"/>
+      <c r="F29" s="72"/>
       <c r="G29" s="43" t="s">
         <v>157</v>
       </c>
@@ -4600,48 +4570,48 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="71">
+      <c r="A30" s="76">
         <v>6</v>
       </c>
-      <c r="B30" s="70" t="s">
+      <c r="B30" s="72" t="s">
         <v>205</v>
       </c>
-      <c r="C30" s="71">
+      <c r="C30" s="76">
         <v>20</v>
       </c>
-      <c r="D30" s="71" t="s">
+      <c r="D30" s="76" t="s">
         <v>136</v>
       </c>
-      <c r="E30" s="70" t="s">
+      <c r="E30" s="72" t="s">
         <v>206</v>
       </c>
-      <c r="F30" s="70"/>
-      <c r="G30" s="68" t="s">
+      <c r="F30" s="72"/>
+      <c r="G30" s="77" t="s">
         <v>207</v>
       </c>
-      <c r="H30" s="68" t="s">
+      <c r="H30" s="77" t="s">
         <v>207</v>
       </c>
-      <c r="I30" s="68" t="s">
+      <c r="I30" s="77" t="s">
         <v>207</v>
       </c>
-      <c r="J30" s="68" t="s">
+      <c r="J30" s="77" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="71"/>
-      <c r="B31" s="70"/>
-      <c r="C31" s="71"/>
-      <c r="D31" s="71"/>
-      <c r="E31" s="70" t="s">
+      <c r="A31" s="76"/>
+      <c r="B31" s="72"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="72" t="s">
         <v>208</v>
       </c>
-      <c r="F31" s="70"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="78"/>
+      <c r="H31" s="78"/>
+      <c r="I31" s="78"/>
+      <c r="J31" s="78"/>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="39">
@@ -4656,10 +4626,10 @@
       <c r="D32" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="E32" s="70" t="s">
+      <c r="E32" s="72" t="s">
         <v>211</v>
       </c>
-      <c r="F32" s="70"/>
+      <c r="F32" s="72"/>
       <c r="G32" s="41" t="s">
         <v>212</v>
       </c>
@@ -4674,50 +4644,50 @@
       </c>
     </row>
     <row r="33" spans="1:10">
-      <c r="A33" s="71">
+      <c r="A33" s="76">
         <v>8</v>
       </c>
-      <c r="B33" s="70" t="s">
+      <c r="B33" s="72" t="s">
         <v>213</v>
       </c>
-      <c r="C33" s="71" t="s">
+      <c r="C33" s="76" t="s">
         <v>214</v>
       </c>
-      <c r="D33" s="71" t="s">
+      <c r="D33" s="76" t="s">
         <v>150</v>
       </c>
       <c r="E33" s="40" t="s">
         <v>215</v>
       </c>
-      <c r="F33" s="70" t="s">
+      <c r="F33" s="72" t="s">
         <v>216</v>
       </c>
-      <c r="G33" s="68" t="s">
+      <c r="G33" s="77" t="s">
         <v>192</v>
       </c>
-      <c r="H33" s="68" t="s">
+      <c r="H33" s="77" t="s">
         <v>192</v>
       </c>
-      <c r="I33" s="68" t="s">
+      <c r="I33" s="77" t="s">
         <v>192</v>
       </c>
-      <c r="J33" s="68" t="s">
+      <c r="J33" s="77" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:10">
-      <c r="A34" s="71"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
+      <c r="A34" s="76"/>
+      <c r="B34" s="72"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="76"/>
       <c r="E34" s="40" t="s">
         <v>217</v>
       </c>
-      <c r="F34" s="70"/>
-      <c r="G34" s="69"/>
-      <c r="H34" s="69"/>
-      <c r="I34" s="69"/>
-      <c r="J34" s="69"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
+      <c r="J34" s="78"/>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="39">
@@ -4732,10 +4702,10 @@
       <c r="D35" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="E35" s="70" t="s">
+      <c r="E35" s="72" t="s">
         <v>220</v>
       </c>
-      <c r="F35" s="70"/>
+      <c r="F35" s="72"/>
       <c r="G35" s="41">
         <v>0</v>
       </c>
@@ -4762,10 +4732,10 @@
       <c r="D36" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="E36" s="70" t="s">
+      <c r="E36" s="72" t="s">
         <v>220</v>
       </c>
-      <c r="F36" s="70"/>
+      <c r="F36" s="72"/>
       <c r="G36" s="41">
         <v>0</v>
       </c>
@@ -4792,8 +4762,8 @@
       <c r="D37" s="39" t="s">
         <v>224</v>
       </c>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
       <c r="G37" s="41" t="s">
         <v>192</v>
       </c>
@@ -4809,21 +4779,33 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="I30:I31"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="H13:H14"/>
@@ -4836,33 +4818,21 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="I30:I31"/>
-    <mergeCell ref="J30:J31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>